<commit_message>
luban export table name to snake case
</commit_message>
<xml_diff>
--- a/datatables/datas/__tables__.xlsx
+++ b/datatables/datas/__tables__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\atom\datatables\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85318622-8655-4CC9-9E3F-0DBCA100EC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E4E968-0F52-4A7A-8A41-E289FE88551F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,13 +103,14 @@
     <t>默认为 &lt;module&gt;_&lt;name&gt;.&lt;suffix&gt;</t>
   </si>
   <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>item.xlsx</t>
+  </si>
+  <si>
     <t>item.TbItem</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>item.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -454,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -562,16 +563,16 @@
     </row>
     <row r="4" spans="1:11">
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>